<commit_message>
Added button position logic to InitialzeExcelDatabases.py
</commit_message>
<xml_diff>
--- a/backend/Excel files/4B.xlsx
+++ b/backend/Excel files/4B.xlsx
@@ -4,19 +4,18 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="January" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="February" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="March" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="April" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="May" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="June" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="July" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="August" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="September" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="October" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="March" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="April" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="May" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="June" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="July" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="August" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="September" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="October" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="November" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,7 +25,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,40 +36,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <color rgb="FFBE0020"/>
-    </font>
-    <font>
-      <color rgb="FF006D08"/>
-    </font>
-    <font>
-      <color rgb="FFA45300"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC1CC"/>
-        <bgColor rgb="FFFFC1CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBAF4CE"/>
-        <bgColor rgb="FFBAF4CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEE97"/>
-        <bgColor rgb="FFFFEE97"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,12 +57,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -770,326 +739,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>NAME</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AADYASHRI GUPTA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AARADHYA JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>AARNA MATHUR</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AATMIKA JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ANANYA MAHIRCHANDANI</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ANAYA VYAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ANVI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ARADHYA GOYAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ARADHYA GURJAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>AROHI KHANDELWAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BHOOMI KHATRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>DIVIJA JOSHI</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>DIVYANSHI</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>DIVYANSHI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>GAURANSHI KHURANA</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>GAURI KAUSHIK</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>GUNJAN JOSHI</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>HARSHITA GUPTA</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>HIRAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>HITANSHI JOGCHAND</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>HIYA GOYAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>KHUSHI JHA</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>KRATI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MANYA KHANDELWAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>MUKTA KHATRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>NAVYA GUPTA</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>NEHAL JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>PAAVANI SHARMA</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>PRANJAL MAHESHWARI</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>RUHEEN KHAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>SAMIKSHA KHANDELWAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>SANVI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>SATVIKA KANKARWAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>SHIVI SETHI</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>SHRASTI KHANGAROT</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>SIDDHI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>SONAKSHI CHANDEL</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>TANVI HIRANI</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>TASHI JAIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>VANSHIKA MAHAWAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>YAJURVI KRISHNATREY</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>YASHIKA KHANDPA</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2376,7 +2025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2390,11 +2039,6 @@
           <t>NAME</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>Jun 24</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2402,11 +2046,6 @@
           <t>AADYASHRI GUPTA</t>
         </is>
       </c>
-      <c r="Y2" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2414,11 +2053,6 @@
           <t>AARADHYA JAIN</t>
         </is>
       </c>
-      <c r="Y3" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2426,11 +2060,6 @@
           <t>AARNA MATHUR</t>
         </is>
       </c>
-      <c r="Y4" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2438,11 +2067,6 @@
           <t>AATMIKA JAIN</t>
         </is>
       </c>
-      <c r="Y5" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2450,11 +2074,6 @@
           <t>ANANYA MAHIRCHANDANI</t>
         </is>
       </c>
-      <c r="Y6" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2462,11 +2081,6 @@
           <t>ANAYA VYAS</t>
         </is>
       </c>
-      <c r="Y7" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2474,11 +2088,6 @@
           <t>ANVI JAIN</t>
         </is>
       </c>
-      <c r="Y8" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2486,11 +2095,6 @@
           <t>ARADHYA GOYAL</t>
         </is>
       </c>
-      <c r="Y9" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2498,11 +2102,6 @@
           <t>ARADHYA GURJAR</t>
         </is>
       </c>
-      <c r="Y10" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2510,11 +2109,6 @@
           <t>AROHI KHANDELWAL</t>
         </is>
       </c>
-      <c r="Y11" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2522,11 +2116,6 @@
           <t>BHOOMI KHATRI</t>
         </is>
       </c>
-      <c r="Y12" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2534,11 +2123,6 @@
           <t>DIVIJA JOSHI</t>
         </is>
       </c>
-      <c r="Y13" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2546,11 +2130,6 @@
           <t>DIVYANSHI</t>
         </is>
       </c>
-      <c r="Y14" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2558,11 +2137,6 @@
           <t>DIVYANSHI JAIN</t>
         </is>
       </c>
-      <c r="Y15" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2570,11 +2144,6 @@
           <t>GAURANSHI KHURANA</t>
         </is>
       </c>
-      <c r="Y16" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2582,11 +2151,6 @@
           <t>GAURI KAUSHIK</t>
         </is>
       </c>
-      <c r="Y17" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2594,11 +2158,6 @@
           <t>GUNJAN JOSHI</t>
         </is>
       </c>
-      <c r="Y18" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2606,11 +2165,6 @@
           <t>HARSHITA GUPTA</t>
         </is>
       </c>
-      <c r="Y19" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2618,11 +2172,6 @@
           <t>HIRAL</t>
         </is>
       </c>
-      <c r="Y20" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2630,11 +2179,6 @@
           <t>HITANSHI JOGCHAND</t>
         </is>
       </c>
-      <c r="Y21" s="4" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2642,11 +2186,6 @@
           <t>HIYA GOYAL</t>
         </is>
       </c>
-      <c r="Y22" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2654,11 +2193,6 @@
           <t>KHUSHI JHA</t>
         </is>
       </c>
-      <c r="Y23" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2666,11 +2200,6 @@
           <t>KRATI JAIN</t>
         </is>
       </c>
-      <c r="Y24" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2678,11 +2207,6 @@
           <t>MANYA KHANDELWAL</t>
         </is>
       </c>
-      <c r="Y25" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2690,11 +2214,6 @@
           <t>MUKTA KHATRI</t>
         </is>
       </c>
-      <c r="Y26" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2702,11 +2221,6 @@
           <t>NAVYA GUPTA</t>
         </is>
       </c>
-      <c r="Y27" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2714,11 +2228,6 @@
           <t>NEHAL JAIN</t>
         </is>
       </c>
-      <c r="Y28" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2726,11 +2235,6 @@
           <t>PAAVANI SHARMA</t>
         </is>
       </c>
-      <c r="Y29" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2738,11 +2242,6 @@
           <t>PRANJAL MAHESHWARI</t>
         </is>
       </c>
-      <c r="Y30" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2750,11 +2249,6 @@
           <t>RUHEEN KHAN</t>
         </is>
       </c>
-      <c r="Y31" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2762,11 +2256,6 @@
           <t>SAMIKSHA KHANDELWAL</t>
         </is>
       </c>
-      <c r="Y32" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2774,11 +2263,6 @@
           <t>SANVI JAIN</t>
         </is>
       </c>
-      <c r="Y33" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2786,11 +2270,6 @@
           <t>SATVIKA KANKARWAL</t>
         </is>
       </c>
-      <c r="Y34" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2798,11 +2277,6 @@
           <t>SHIVI SETHI</t>
         </is>
       </c>
-      <c r="Y35" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2810,11 +2284,6 @@
           <t>SHRASTI KHANGAROT</t>
         </is>
       </c>
-      <c r="Y36" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2822,11 +2291,6 @@
           <t>SIDDHI JAIN</t>
         </is>
       </c>
-      <c r="Y37" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2834,11 +2298,6 @@
           <t>SONAKSHI CHANDEL</t>
         </is>
       </c>
-      <c r="Y38" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2846,11 +2305,6 @@
           <t>TANVI HIRANI</t>
         </is>
       </c>
-      <c r="Y39" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2858,11 +2312,6 @@
           <t>TASHI JAIN</t>
         </is>
       </c>
-      <c r="Y40" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2870,11 +2319,6 @@
           <t>VANSHIKA MAHAWAR</t>
         </is>
       </c>
-      <c r="Y41" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2882,21 +2326,11 @@
           <t>YAJURVI KRISHNATREY</t>
         </is>
       </c>
-      <c r="Y42" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
           <t>YASHIKA KHANDPA</t>
-        </is>
-      </c>
-      <c r="Y43" s="2" t="inlineStr">
-        <is>
-          <t>P</t>
         </is>
       </c>
     </row>

</xml_diff>